<commit_message>
added new problems on linked list to the sheet
</commit_message>
<xml_diff>
--- a/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
+++ b/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aswithkumarcheella/Personal_documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aswithkumarcheella/Developer/Leetcode_solutions/Leetcode Prolems Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9514A7-F175-3247-9C07-2A5D40D862C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5E514-5C92-944A-83C2-947B06578334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="834">
   <si>
     <t>Problem number</t>
   </si>
@@ -6432,6 +6432,136 @@
   <si>
     <t>The solution merges two singly-linked lists list1 and list2 by replacing a segment of list1 from position a to b with the entire list2. It iterates through list1 to identify the nodes just before position a (edge1) and right after b (edge2). I
 t then traverses list2 to reach its last node, linking this last node to edge2. Finally, edge1.next is linked to the head of list2, effectively merging list2 into list1 and returning the modified list1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def removeNodes(self, head: Optional[ListNode]) -&gt; Optional[ListNode]:
+        #monotonic stack approach
+        # stack = []
+        # cur = head
+        # while cur:
+        #     while stack and cur.val &gt; stack[-1]:
+        #         stack.pop()
+        #     stack.append(cur.val)
+        #     cur = cur.next
+        # #build the linkedlist with the remaining node
+        # dummy = ListNode()
+        # cur = dummy
+        # for n in stack:
+        #     cur.next = ListNode(n)
+        #     cur = cur.next
+        # return dummy.next
+        #reverse the linkedlist
+        def reverse(head):
+            prev, cur = None, head
+            while cur:
+                nxt = cur.next
+                cur.next = prev
+                prev = cur
+                cur = nxt
+            return prev
+        #prev is now head of the reversed linked list
+        head = reverse(head)
+        cur = head
+        cur_max = cur.val
+        while cur.next:
+            if cur.next.val &lt; cur_max:
+                cur.next = cur.next.next
+            else:
+                cur_max = cur.next.val
+                cur = cur.next
+        return reverse(head)
+        </t>
+  </si>
+  <si>
+    <t>Remove Nodes From Linked List</t>
+  </si>
+  <si>
+    <t>The provided solution removes nodes from a singly-linked list that are less than any node occurring later in the list, using a reversed list approach.
+	1.	The list is first reversed to process nodes in reverse order.
+	2.	While traversing the reversed list, a maximum value (cur_max) is maintained, and nodes with values less than cur_max are skipped.
+	3.	If a node’s value is greater than or equal to cur_max, the maximum is updated, and traversal continues.
+	4.	The list is reversed again to restore the original order with only the desired nodes retained.
+	5.	The resulting linked list is returned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def pairSum(self, head: Optional[ListNode]) -&gt; int:
+        #find middle using slow and fast pointers
+        slow, fast = head, head.next
+        while fast and fast.next:
+            slow = slow.next
+            fast = fast.next.next
+        #reverse second half of the list
+        second = slow.next
+        slow.next = None
+        prev = None
+        while second:
+            nxt = second.next
+            second.next = prev
+            prev = second
+            second = nxt
+        left, right = head, prev
+        max_sum = 0
+        while right:
+            twin_sum = left.val + right.val
+            max_sum = max(max_sum, twin_sum)
+            left = left.next
+            right = right.next
+        return max_sum
+    </t>
+  </si>
+  <si>
+    <t>Maximum Twin Sum of a Linked List</t>
+  </si>
+  <si>
+    <t>The solution finds the maximum twin sum of a linked list using a two-step process:
+	1.	Finding the middle: It uses the slow and fast pointer technique to locate the middle of the list, where slow points to the middle node when fast reaches the end.
+	2.	Reversing the second half: The list’s second half is reversed in place to make it easier to calculate twin sums from both ends.
+	3.	Calculating twin sums: It traverses both halves simultaneously, calculating the sum of paired nodes from the start and end, and keeps track of the maximum twin sum.
+	4.	Finally, the maximum twin sum is returned.
+This approach is efficient, with a time complexity of O(n) and space complexity of O(1).</t>
+  </si>
+  <si>
+    <t># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def swapNodes(self, head: Optional[ListNode], k: int) -&gt; Optional[ListNode]:
+        cur = head
+        for i in range(k-1):
+            cur = cur.next
+        left = cur
+        right = head
+        while cur.next:
+            cur = cur.next
+            right = right.next
+        #swap left and right values
+        left.val, right.val = right.val, left.val
+        return head</t>
+  </si>
+  <si>
+    <t>Swapping Nodes in a Linked List</t>
+  </si>
+  <si>
+    <t>The solution swaps the values of two nodes in a singly-linked list at positions k from the beginning and k from the end:
+	1.	It first traverses to the k-th node from the beginning (left node) using a simple loop.
+	2.	It then uses two pointers: cur to continue from the k-th node and right starting from head, moving both until cur reaches the end. This positions right at the k-th node from the end.
+	3.	The values of the left and right nodes are swapped.
+	4.	Finally, the modified list is returned.
+This approach ensures efficient traversal in O(n) time with O(1) space.</t>
   </si>
 </sst>
 </file>
@@ -6640,7 +6770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6715,6 +6845,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7225,8 +7358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D222" sqref="D222"/>
+    <sheetView tabSelected="1" topLeftCell="A225" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D225" sqref="D225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.6640625" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -23069,13 +23202,25 @@
       <c r="BP222" s="8"/>
       <c r="BQ222" s="8"/>
     </row>
-    <row r="223" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A223" s="8"/>
-      <c r="B223" s="8"/>
-      <c r="C223" s="8"/>
-      <c r="D223" s="8"/>
-      <c r="E223" s="8"/>
-      <c r="F223" s="8"/>
+    <row r="223" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>2487</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F223" s="3" t="s">
+        <v>825</v>
+      </c>
       <c r="G223" s="8"/>
       <c r="H223" s="8"/>
       <c r="I223" s="8"/>
@@ -23140,13 +23285,25 @@
       <c r="BP223" s="8"/>
       <c r="BQ223" s="8"/>
     </row>
-    <row r="224" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A224" s="8"/>
-      <c r="B224" s="8"/>
-      <c r="C224" s="8"/>
-      <c r="D224" s="8"/>
-      <c r="E224" s="8"/>
-      <c r="F224" s="8"/>
+    <row r="224" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>2130</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>828</v>
+      </c>
       <c r="G224" s="8"/>
       <c r="H224" s="8"/>
       <c r="I224" s="8"/>
@@ -23211,13 +23368,25 @@
       <c r="BP224" s="8"/>
       <c r="BQ224" s="8"/>
     </row>
-    <row r="225" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A225" s="8"/>
-      <c r="B225" s="8"/>
-      <c r="C225" s="8"/>
-      <c r="D225" s="8"/>
-      <c r="E225" s="8"/>
-      <c r="F225" s="8"/>
+    <row r="225" spans="1:69" ht="320" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>1721</v>
+      </c>
+      <c r="B225" s="28" t="s">
+        <v>832</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>831</v>
+      </c>
       <c r="G225" s="8"/>
       <c r="H225" s="8"/>
       <c r="I225" s="8"/>
@@ -55732,13 +55901,14 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B172" r:id="rId1" display="https://leetcode.com/problems/valid-palindrome-ii/" xr:uid="{1F43B8A8-BD5E-432E-93F6-CAD7210F25EE}"/>
+    <hyperlink ref="B225" r:id="rId2" display="https://leetcode.com/problems/swapping-nodes-in-a-linked-list/" xr:uid="{F34C9997-11A2-B148-82EE-103F6B2DE36C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000  &amp;1#_x000D_</oddHeader>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added few more linkedlist problems
</commit_message>
<xml_diff>
--- a/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
+++ b/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aswithkumarcheella/Developer/Leetcode_solutions/Leetcode Prolems Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5E514-5C92-944A-83C2-947B06578334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E37E578-DA7B-B242-952C-B3BC00FB4064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="855">
   <si>
     <t>Problem number</t>
   </si>
@@ -6562,6 +6562,253 @@
 	3.	The values of the left and right nodes are swapped.
 	4.	Finally, the modified list is returned.
 This approach ensures efficient traversal in O(n) time with O(1) space.</t>
+  </si>
+  <si>
+    <t>"""
+# Definition for a Node.
+class Node:
+    def __init__(self, x: int, next: 'Node' = None, random: 'Node' = None):
+        self.val = int(x)
+        self.next = next
+        self.random = random
+"""
+class Solution:
+    def copyRandomList(self, head: 'Optional[Node]') -&gt; 'Optional[Node]':
+        #track old to new nodes using a hashmap
+        oldToCopy = {None: None}
+        cur = head
+        while cur:
+            copy = Node(cur.val)
+            oldToCopy[cur] = copy
+            cur = cur.next
+        cur = head
+        while cur:
+            copy = oldToCopy[cur]
+            copy.next = oldToCopy[cur.next]
+            copy.random = oldToCopy[cur.random]
+            cur = cur.next
+        return oldToCopy[head]</t>
+  </si>
+  <si>
+    <t>The solution creates a deep copy of a linked list where each node has a next pointer and a random pointer using a hashmap:
+	1.	Mapping nodes: It iterates through the original list, creating a copy of each node and storing these in a dictionary oldToCopy, which maps each original node to its copy. This mapping allows easy access to the new node corresponding to any old node, including handling None as a key for clarity.
+	2.	Assigning pointers: A second pass through the original list assigns the next and random pointers for each copied node using the oldToCopy dictionary. This ensures that the copied nodes have the correct relationships.
+	3.	The copied head node is then returned, providing a fully deep-copied list structure.
+This approach runs in O(n) time and uses O(n) space for the hashmap.</t>
+  </si>
+  <si>
+    <t>class Node:
+    def __init__(self, val = 0, next = None, prev = None):
+        self.val = val
+        self.next = next
+        self.prev = prev
+class MyLinkedList:
+    def __init__(self):
+        self.size = 0
+        self.head, self.tail = Node(), Node()
+        self.head.next = self.tail
+        self.tail.prev = self.head
+    def get(self, index: int) -&gt; int:
+        if index &gt;= self.size: # invalid index
+            return -1
+        cur = self.head
+        for _ in range(index+1):
+            cur = cur.next
+        return cur.val
+    def addAtHead(self, val: int) -&gt; None:
+        self.addAtIndex(0, val)
+    def addAtTail(self, val: int) -&gt; None:
+        self.addAtIndex(self.size, val)
+    def addAtIndex(self, index: int, val: int) -&gt; None:
+        if index &gt; self.size:  # invalid index
+            return
+        prev = self.head
+        for _ in range(index):
+            prev = prev.next
+        # insert `newNode` between `prev` and `prev.next`
+        newNode = Node(val, prev.next, prev)
+        prev.next.prev = newNode
+        prev.next = newNode
+        self.size += 1
+    def deleteAtIndex(self, index: int) -&gt; None:
+        if index &gt;= self.size:  # invalid index
+            return
+        prev = self.head
+        for _ in range(index):
+            prev = prev.next
+        nxt = prev.next.next
+        prev.next = nxt
+        nxt.prev = prev
+        self.size -= 1</t>
+  </si>
+  <si>
+    <t>Design Linked List</t>
+  </si>
+  <si>
+    <t>Here’s a clearer explanation with additional details for each step:
+	1.	Initialization (__init__):
+	•	The MyLinkedList class initializes with two sentinel nodes, head and tail, that make it easier to handle edge cases like adding or removing nodes at the boundaries.
+	•	head.next points to tail, and tail.prev points to head, creating a dummy structure to simplify pointer updates during insertions and deletions. The initial size of the list is set to 0.
+	2.	get(index):
+	•	This method retrieves the value at the specified index by traversing the list from the head. It stops at the desired position, skipping index + 1 nodes, since the head sentinel does not hold a value.
+	•	If the provided index is greater than or equal to the size of the list (indicating an invalid index), the method returns -1. Otherwise, it returns the value of the node at that index.
+	3.	addAtHead(val) and addAtTail(val):
+	•	addAtHead(val) inserts a new node at the beginning of the list by calling addAtIndex(0, val), effectively placing the value right after the head sentinel.
+	•	addAtTail(val) inserts a new node at the end of the list by calling addAtIndex(self.size, val), adding the value just before the tail sentinel, ensuring consistent behavior for both operations.
+	4.	addAtIndex(index, val):
+	•	This method inserts a new node at the specified index. If the index is greater than the current size, it does nothing (invalid index case). However, if the index equals the size, the node is appended at the tail.
+	•	To insert, it first locates the node at the given index by traversing from the head. It then creates a new node and adjusts the next and prev pointers of neighboring nodes to include the new node, increasing the list size by 1.
+	5.	deleteAtIndex(index):
+	•	This method removes the node at the specified index. If the index is invalid (greater than or equal to the size), the operation is ignored to avoid errors.
+	•	If valid, it traverses to the node just before the one to be removed. It then adjusts pointers to skip the node being deleted, linking the previous and next nodes directly to each other and reducing the list size by 1.
+Overall, this implementation ensures efficient management of nodes in a doubly-linked list, providing O(1) operations for adding or removing elements at the head or tail, and O(n) operations for arbitrary index access, insertion, and deletion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time: O(1) adding and removing, O(N) for adding at index </t>
+  </si>
+  <si>
+    <t># class ListNode:
+#     def __init__(self, val, prev=None, next=None):
+#         self.val = val
+#         self.prev = prev
+#         self.next = next
+class BrowserHistory:
+    def __init__(self, homepage: str):
+        # self.cur = ListNode(homepage)
+        self.i = 0
+        self.len = 1
+        self.browser = [homepage]
+    def visit(self, url: str) -&gt; None:
+        # self.cur.next = ListNode(url, prev=self.cur)
+        # self.cur = self.cur.next
+        if len(self.browser) &lt; self.i + 2:
+            self.browser.append(url)
+        else:
+            self.browser[self.i + 1] = url
+        self.i += 1
+        self.len = self.i + 1
+    def back(self, steps: int) -&gt; str:
+        # while self.cur.prev and steps &gt; 0:
+        #     self.cur = self.cur.prev
+        #     steps -= 1
+        # return self.cur.val
+        self.i = max(self.i - steps, 0)
+        return self.browser[self.i]
+    def forward(self, steps: int) -&gt; str:
+        # while self.cur.next and steps &gt; 0:
+        #     self.cur = self.cur.next
+        #     steps -= 1
+        # return self.cur.val
+        self.i = min(self.i + steps, self.len - 1)
+        return self.browser[self.i]
+# Your BrowserHistory object will be instantiated and called as such:
+# obj = BrowserHistory(homepage)
+# obj.visit(url)
+# param_2 = obj.back(steps)
+# param_3 = obj.forward(steps)</t>
+  </si>
+  <si>
+    <t>Linked List/Dynamic Array</t>
+  </si>
+  <si>
+    <t>Design Browser History</t>
+  </si>
+  <si>
+    <t>The BrowserHistory class simulates a simplified browser history feature using a list to manage visited URLs and integer indices to track the current position. Here’s a detailed explanation of each method:
+	1.	Initialization (__init__):
+	•	The constructor initializes the browser history with the given homepage. It uses a list, self.browser, to store URLs, starting with the homepage.
+	•	self.i tracks the current index in the history, and self.len keeps track of the valid length of the history, which is initially 1 (the homepage).
+	2.	visit(url):
+	•	This method is called when visiting a new URL. If necessary, it appends the new URL to the history list, or it overwrites the next position if the browser history has been previously truncated by moving back.
+	•	After visiting a new URL, self.i is updated to point to the newly visited URL, and self.len is adjusted to reflect the new length of the history, removing any future history.
+	3.	back(steps):
+	•	This method moves backward in the browser history by steps, but it does not move beyond the start of the history. self.i is adjusted to the maximum of self.i - steps and 0 to ensure it stays within bounds.
+	•	It then returns the URL at the current index, self.browser[self.i].
+	4.	forward(steps):
+	•	This method moves forward in the browser history by steps, but it does not move past the most recently visited URL. self.i is adjusted to the minimum of self.i + steps and self.len - 1 to stay within bounds.
+	•	It returns the URL at the current index, self.browser[self.i].
+Key Points:
+	•	The implementation efficiently manages browser history using a list and integer indices, achieving O(1) time complexity for each operation.
+	•	The visit method truncates any forward history beyond the current point, mimicking the behavior of a real browser.
+	•	back and forward ensure the indices remain within valid bounds to prevent errors.
+This design is simpler and more efficient than using a doubly-linked list for the given operations, with the list structure providing easy access to history URLs.</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def hasIncreasingSubarrays(self, nums: List[int], k: int) -&gt; bool:
+        n = len(nums)
+        dp = [1] * n
+        for i in range(n - 2, -1, -1):
+            if nums[i] &lt; nums[i + 1]:
+                dp[i] = 1 + dp[i + 1]
+        for i in range(n - 2 * k + 1):
+            if dp[i] &gt;= k and dp[i + k] &gt;= k:
+                return True
+        return False</t>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Adjacent Increasing Subarrays Detection I</t>
+  </si>
+  <si>
+    <t>Q1(11/10/2024)</t>
+  </si>
+  <si>
+    <t>The given solution checks if there exist two non-overlapping subarrays of length  k  with strictly increasing elements in the list nums. It initializes a list dp where each element denotes the length of the longest increasing suffix starting from that position. The code iterates backward to populate dp based on whether the next element is greater. Then, it checks for indices i where two subarrays starting at i and i + k both have a length of at least  k . 
+If such subarrays are found, it returns True; otherwise, it returns False.</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def maxIncreasingSubarrays(self, nums: List[int]) -&gt; int:
+        def hasIncreasingSubarrays(nums: List[int], k: int) -&gt; bool:
+            n = len(nums)
+            dp = [1] * n
+            for i in range(n - 2, -1, -1):
+                if nums[i] &lt; nums[i + 1]:
+                    dp[i] = 1 + dp[i + 1]
+            for i in range(n - 2 * k + 1):
+                if dp[i] &gt;= k and dp[i + k] &gt;= k:
+                    return True
+            return False
+        l, r = 1, len(nums) // 2
+        while l &lt;= r:
+            m = (l + r) // 2
+            if hasIncreasingSubarrays(nums, m): l = m + 1
+            else: r = m - 1
+        return r</t>
+  </si>
+  <si>
+    <t>Dynamic Programming/Binary Search</t>
+  </si>
+  <si>
+    <t>Adjacent Increasing Subarrays Detection II</t>
+  </si>
+  <si>
+    <t>Q2(11/10/2024)</t>
+  </si>
+  <si>
+    <t>3.	Helper Function (hasIncreasingSubarrays):
+	•	Computes the longest increasing suffix lengths using a dynamic programming (DP) array dp.
+	•	Iterates backward through nums to populate dp, where dp[i] indicates the length of the increasing subarray starting from index  i .
+	4.	Subarray Check: The helper function then checks if there are two non-overlapping subarrays of length  k  by comparing values in dp at positions  i  and  i + k .
+	5.	Binary Search Setup: The main function uses binary search to efficiently determine the maximum  k . It initializes l as 1 and r as half the length of nums.
+	6.	Binary Search Loop: The loop runs until l exceeds r, calculating the midpoint  m  and using hasIncreasingSubarrays to check for subarrays of length  m .
+	7.	Adjusting Bounds: If the subarrays of length  m  exist, it increases the lower bound l to search for a larger  k ; otherwise, it decreases the upper bound r.
+	8.	Return Value: The function returns r, the maximum  k  where two such subarrays are still possible.
+	9.	Efficiency: The use of binary search reduces the time complexity compared to a linear scan, making the solution more efficient.
+	10.	Overall Complexity: The solution efficiently combines dynamic programming and binary search to solve the problem with reduced time complexity compared to a brute-force approach.</t>
+  </si>
+  <si>
+    <t>This solution uses Floyd’s Tortoise and Hare (Cycle Detection) algorithm to find a duplicate number in an array. Here’s the explanation:
+	1.	Initialize two pointers, slow and fast, both starting at the first element of nums.
+	2.	Move slow one step at a time and fast two steps at a time, creating a scenario similar to detecting a cycle in a linked list.
+	3.	Continue moving slow and fast until they meet, indicating the presence of a cycle.
+	4.	Once a cycle is detected, initialize a new pointer slow2 at the beginning of nums.
+	5.	Move both slow and slow2 one step at a time until they meet again.
+	6.	The meeting point is the duplicate number, which is returned.
+	7.	This approach uses constant space (O(1)) and runs in linear time (O(n)).</t>
   </si>
 </sst>
 </file>
@@ -7358,8 +7605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D225" sqref="D225"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.6640625" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -12440,8 +12687,12 @@
       <c r="C93" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
+      <c r="D93" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F93" s="3" t="s">
         <v>337</v>
       </c>
@@ -23451,13 +23702,25 @@
       <c r="BP225" s="8"/>
       <c r="BQ225" s="8"/>
     </row>
-    <row r="226" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A226" s="8"/>
-      <c r="B226" s="8"/>
-      <c r="C226" s="8"/>
-      <c r="D226" s="8"/>
-      <c r="E226" s="8"/>
-      <c r="F226" s="8"/>
+    <row r="226" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>138</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F226" s="3" t="s">
+        <v>834</v>
+      </c>
       <c r="G226" s="8"/>
       <c r="H226" s="8"/>
       <c r="I226" s="8"/>
@@ -23522,13 +23785,25 @@
       <c r="BP226" s="8"/>
       <c r="BQ226" s="8"/>
     </row>
-    <row r="227" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A227" s="8"/>
-      <c r="B227" s="8"/>
-      <c r="C227" s="8"/>
-      <c r="D227" s="8"/>
-      <c r="E227" s="8"/>
-      <c r="F227" s="8"/>
+    <row r="227" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>707</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="F227" s="3" t="s">
+        <v>836</v>
+      </c>
       <c r="G227" s="8"/>
       <c r="H227" s="8"/>
       <c r="I227" s="8"/>
@@ -23593,13 +23868,25 @@
       <c r="BP227" s="8"/>
       <c r="BQ227" s="8"/>
     </row>
-    <row r="228" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A228" s="8"/>
-      <c r="B228" s="8"/>
-      <c r="C228" s="8"/>
-      <c r="D228" s="8"/>
-      <c r="E228" s="8"/>
-      <c r="F228" s="8"/>
+    <row r="228" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>1472</v>
+      </c>
+      <c r="B228" s="28" t="s">
+        <v>842</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F228" s="3" t="s">
+        <v>840</v>
+      </c>
       <c r="G228" s="8"/>
       <c r="H228" s="8"/>
       <c r="I228" s="8"/>
@@ -23664,13 +23951,25 @@
       <c r="BP228" s="8"/>
       <c r="BQ228" s="8"/>
     </row>
-    <row r="229" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A229" s="8"/>
-      <c r="B229" s="8"/>
-      <c r="C229" s="8"/>
-      <c r="D229" s="8"/>
-      <c r="E229" s="8"/>
-      <c r="F229" s="8"/>
+    <row r="229" spans="1:69" ht="176" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>844</v>
+      </c>
       <c r="G229" s="8"/>
       <c r="H229" s="8"/>
       <c r="I229" s="8"/>
@@ -23735,13 +24034,25 @@
       <c r="BP229" s="8"/>
       <c r="BQ229" s="8"/>
     </row>
-    <row r="230" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A230" s="8"/>
-      <c r="B230" s="8"/>
-      <c r="C230" s="8"/>
-      <c r="D230" s="8"/>
-      <c r="E230" s="8"/>
-      <c r="F230" s="8"/>
+    <row r="230" spans="1:69" ht="304" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>849</v>
+      </c>
       <c r="G230" s="8"/>
       <c r="H230" s="8"/>
       <c r="I230" s="8"/>
@@ -55902,13 +56213,14 @@
   <hyperlinks>
     <hyperlink ref="B172" r:id="rId1" display="https://leetcode.com/problems/valid-palindrome-ii/" xr:uid="{1F43B8A8-BD5E-432E-93F6-CAD7210F25EE}"/>
     <hyperlink ref="B225" r:id="rId2" display="https://leetcode.com/problems/swapping-nodes-in-a-linked-list/" xr:uid="{F34C9997-11A2-B148-82EE-103F6B2DE36C}"/>
+    <hyperlink ref="B228" r:id="rId3" display="https://leetcode.com/problems/design-browser-history/" xr:uid="{AFC68F7D-3724-7846-A3E1-FED24827FDDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000  &amp;1#_x000D_</oddHeader>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added few more linked list problems
</commit_message>
<xml_diff>
--- a/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
+++ b/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aswithkumarcheella/Developer/Leetcode_solutions/Leetcode Prolems Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E37E578-DA7B-B242-952C-B3BC00FB4064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7FDCAC-D2F8-7A45-944B-02CA11BE6B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="868">
   <si>
     <t>Problem number</t>
   </si>
@@ -6809,6 +6809,191 @@
 	5.	Move both slow and slow2 one step at a time until they meet again.
 	6.	The meeting point is the duplicate number, which is returned.
 	7.	This approach uses constant space (O(1)) and runs in linear time (O(n)).</t>
+  </si>
+  <si>
+    <t># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def swapPairs(self, head: Optional[ListNode]) -&gt; Optional[ListNode]:
+        dummy = ListNode(0, head)
+        prev, curr = dummy, head
+        #only proceed to swap if atleast two nodes are present
+        while curr and curr.next:
+            #save pointers
+            nxtPair = curr.next.next
+            second = curr.next
+            #reverse nodes curr and second
+            second.next = curr
+            curr.next = nxtPair
+            prev.next = second
+            #update pointers
+            prev = curr
+            curr = nxtPair
+        return dummy.next</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>This solution swaps every two adjacent nodes in a linked list and returns the modified list. Here’s the breakdown:
+	1.	Create a dummy node, dummy, that points to the head of the list. This helps handle edge cases cleanly.
+	2.	Initialize prev to dummy and curr to the head of the list.
+	3.	Use a while loop to swap nodes only if at least two nodes (curr and curr.next) are available.
+	4.	Save pointers to the next pair (nxtPair) and the second node (second) in the pair to be swapped.
+	5.	Reverse the nodes: point second.next to curr, and curr.next to nxtPair.
+	6.	Adjust prev.next to point to second, completing the swap for the current pair.
+	7.	Move prev to curr and curr to nxtPair to proceed to the next pair of nodes.
+	8.	Return dummy.next, which is the new head of the modified list.
+	9.	The solution runs in linear time (O(n)) and uses constant space (O(1)).</t>
+  </si>
+  <si>
+    <t># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def sortList(self, head: Optional[ListNode]) -&gt; Optional[ListNode]:
+        if not head or not head.next:
+            return head
+        left = head
+        right = self.getMid(head)
+        tmp = right.next
+        right.next = None
+        right = tmp
+        left = self.sortList(left)
+        right = self.sortList(right)
+        return self.merge(left, right)
+    def getMid(self, head):
+        slow, fast = head, head.next
+        while fast and fast.next:
+            slow = slow.next
+            fast = fast.next.next
+        return slow
+    def merge(self, l1, l2):
+        tail = dummy = ListNode()
+        while l1 and l2:
+            if l1.val &lt; l2.val:
+                tail.next = l1
+                l1 = l1.next
+            else:
+                tail.next = l2
+                l2 = l2.next
+            tail = tail.next
+        if l1:
+            tail.next = l1
+        elif l2:
+            tail.next = l2
+        return dummy.next</t>
+  </si>
+  <si>
+    <t>Sorted List</t>
+  </si>
+  <si>
+    <t>This solution sorts a linked list using the Merge Sort algorithm. Here’s how it works:
+	1.	Base Case: If the list is empty or has only one node, return head as it’s already sorted.
+	2.	Split the List: Use the getMid function to find the middle of the list, splitting it into two halves: left and right.
+	•	getMid uses the two-pointer technique (slow and fast) to find the middle node efficiently.
+	3.	Recursively Sort: Recursively call sortList on both halves (left and right) to sort them.
+	4.	Merge Sorted Halves: Use the merge function to merge the two sorted halves.
+	•	The merge function uses a dummy node to facilitate the merging process, comparing values from l1 and l2 and building a sorted list.
+	5.	Return the Sorted List: The merge function returns dummy.next, which is the head of the merged and sorted list.
+	6.	Complexity: The time complexity is O(n log n) due to the divide-and-conquer approach, and the space complexity is O(log n) for the recursive call stack.</t>
+  </si>
+  <si>
+    <t>Time: O(NlogN)
+Space: O(logN)</t>
+  </si>
+  <si>
+    <t># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def partition(self, head: Optional[ListNode], x: int) -&gt; Optional[ListNode]:
+        left, right = ListNode(), ListNode()
+        ltail, rtail = left, right
+        while head:
+            if head.val &lt; x:
+                ltail.next = head
+                ltail = ltail.next
+            else:
+                rtail.next = head
+                rtail = rtail.next
+            head = head.next
+        ltail.next = right.next
+        rtail.next = None
+        return left.next</t>
+  </si>
+  <si>
+    <t>Partition List</t>
+  </si>
+  <si>
+    <t>1.	Initialize Two Linked Lists:
+	•	Two dummy nodes, left and right, are created to form two separate linked lists: one for nodes with values less than x and the other for nodes with values greater than or equal to x.
+	•	ltail and rtail are pointers that will help build these two lists.
+	2.	Traverse the Original Linked List:
+	•	Iterate through the given linked list node by node.
+	•	If the current node’s value is less than x, append it to the left list, and move ltail to this new node.
+	•	Otherwise, append it to the right list, and move rtail to this new node.
+	3.	Combine the Two Lists:
+	•	The left list’s tail (ltail) is connected to the head of the right list (right.next), which combines both partitions.
+	•	rtail.next is set to None to ensure the new linked list ends properly.
+	4.	Return the Partitioned List:
+	•	Return left.next as the head of the partitioned list, skipping the dummy node at the start of the left list.</t>
+  </si>
+  <si>
+    <t># Definition for singly-linked list.
+# class ListNode:
+#     def __init__(self, val=0, next=None):
+#         self.val = val
+#         self.next = next
+class Solution:
+    def rotateRight(self, head: Optional[ListNode], k: int) -&gt; Optional[ListNode]:
+        if not head:
+            return head
+        length, tail = 1, head
+        while tail.next:
+            tail = tail.next
+            length += 1
+        k = k % length
+        if k == 0:
+            return head
+        cur = head
+        for i in range(length - k - 1):
+            cur = cur.next
+        newHead = cur.next
+        cur.next = None
+        tail.next = head
+        return newHead</t>
+  </si>
+  <si>
+    <t>Rotate List</t>
+  </si>
+  <si>
+    <t>The code provided rotates a linked list to the right by k positions, where k can be any non-negative integer. Here’s a breakdown of how the algorithm works:
+	1.	Handle Edge Cases:
+	•	If the linked list is empty (head is None), the function simply returns head.
+	•	This early return handles cases where no rotation is necessary.
+	2.	Calculate the Length of the Linked List:
+	•	length is initialized to 1, and tail starts at the head node.
+	•	A loop iterates through the linked list to find the last node (tail) and calculate the total length.
+	3.	Adjust k to Avoid Redundant Rotations:
+	•	k is updated using k % length to ensure we do not rotate the list unnecessarily. If k is a multiple of length, the list remains unchanged.
+	4.	Return Early If No Rotation Is Needed:
+	•	If k becomes 0 after the modulus operation, the function returns head, as the list does not need to be rotated.
+	5.	Locate the New Head:
+	•	Using length - k - 1, the code finds the node (cur) that will become the last node after rotation.
+	•	The new head will be the node immediately following cur.
+	6.	Rearrange Pointers to Rotate:
+	•	cur.next is set to None to terminate the list at the new last node.
+	•	tail.next is linked to the old head to complete the rotation.
+	7.	Return the New Head:
+	•	The new head of the rotated list (newHead) is returned.</t>
   </si>
 </sst>
 </file>
@@ -7605,8 +7790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A234" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B234" sqref="B234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.6640625" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -24117,13 +24302,25 @@
       <c r="BP230" s="8"/>
       <c r="BQ230" s="8"/>
     </row>
-    <row r="231" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A231" s="8"/>
-      <c r="B231" s="8"/>
-      <c r="C231" s="8"/>
-      <c r="D231" s="8"/>
-      <c r="E231" s="8"/>
-      <c r="F231" s="8"/>
+    <row r="231" spans="1:69" ht="395" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>24</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>855</v>
+      </c>
       <c r="G231" s="8"/>
       <c r="H231" s="8"/>
       <c r="I231" s="8"/>
@@ -24188,13 +24385,25 @@
       <c r="BP231" s="8"/>
       <c r="BQ231" s="8"/>
     </row>
-    <row r="232" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A232" s="8"/>
-      <c r="B232" s="8"/>
-      <c r="C232" s="8"/>
-      <c r="D232" s="8"/>
-      <c r="E232" s="8"/>
-      <c r="F232" s="8"/>
+    <row r="232" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
+        <v>148</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>858</v>
+      </c>
       <c r="G232" s="8"/>
       <c r="H232" s="8"/>
       <c r="I232" s="8"/>
@@ -24259,13 +24468,25 @@
       <c r="BP232" s="8"/>
       <c r="BQ232" s="8"/>
     </row>
-    <row r="233" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A233" s="8"/>
-      <c r="B233" s="8"/>
-      <c r="C233" s="8"/>
-      <c r="D233" s="8"/>
-      <c r="E233" s="8"/>
-      <c r="F233" s="8"/>
+    <row r="233" spans="1:69" ht="320" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>86</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F233" s="3" t="s">
+        <v>862</v>
+      </c>
       <c r="G233" s="8"/>
       <c r="H233" s="8"/>
       <c r="I233" s="8"/>
@@ -24330,13 +24551,25 @@
       <c r="BP233" s="8"/>
       <c r="BQ233" s="8"/>
     </row>
-    <row r="234" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A234" s="8"/>
-      <c r="B234" s="8"/>
-      <c r="C234" s="8"/>
-      <c r="D234" s="8"/>
-      <c r="E234" s="8"/>
-      <c r="F234" s="8"/>
+    <row r="234" spans="1:69" ht="380" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>61</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F234" s="3" t="s">
+        <v>865</v>
+      </c>
       <c r="G234" s="8"/>
       <c r="H234" s="8"/>
       <c r="I234" s="8"/>
@@ -56226,20 +56459,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="65e36ddc-5285-4041-8458-a3fe69788910" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="65e36ddc-5285-4041-8458-a3fe69788910" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56490,6 +56723,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{212D311D-CC3C-415A-BAF4-A187391AFDAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC15491-6D28-440E-AD32-C4EA2153CE82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -56502,14 +56743,6 @@
     <ds:schemaRef ds:uri="65e36ddc-5285-4041-8458-a3fe69788910"/>
     <ds:schemaRef ds:uri="fe9ba8f0-2b3b-40f1-8ad7-a301ec5c98cd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{212D311D-CC3C-415A-BAF4-A187391AFDAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
leetcode weekly contest problems added
</commit_message>
<xml_diff>
--- a/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
+++ b/Leetcode Prolems Sheet/Leetcode Prolems.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aswithkumarcheella/Developer/Leetcode_solutions/Leetcode Prolems Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212E7317-8A9F-C94B-BC65-DEBE28C4FFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A915B4-07E0-3D4E-94C5-17F66DBD67C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="882">
   <si>
     <t>Problem number</t>
   </si>
@@ -7040,6 +7040,122 @@
 	•	leftprev.next is updated to prev to link the start of the list to the new head of the reversed section.
 	5.	Return the Modified List:
 	•	dummy.next is returned as the new head of the modified list.</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def isZeroArray(self, nums: List[int], queries: List[List[int]]) -&gt; bool:
+        # #brute force approach
+        # for l, r in queries:
+        #     for i in range(l, r + 1):
+        #         if nums[i] != 0:
+        #             nums[i] -= 1
+        # #nums = [1, 0, 0, 0, 0]
+        # for i in range(len(nums)):
+        #     if nums[i] != 0:
+        #         return False
+        # return True
+        n = len(nums)
+        diff = [0]*(n+1)
+        #diff = [0, 0, 0, 0, 0] #n+1 length
+        for start, end in queries:
+            diff[start] += 1
+            diff[end+1] -= 1
+        ops = 0
+        for i in range(len(nums)):
+            ops += diff[i]
+            if ops &lt; nums[i]:
+                return False
+        return True</t>
+  </si>
+  <si>
+    <t>Arrays and Prefix sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	1.	Initialize Difference Array:
+	•	We create a difference array diff of size n + 1, initialized with zeros, where n is the length of nums.
+	•	diff will help to track the cumulative effect of decrement operations.
+	2.	Apply Operations Using Difference Array:
+	•	Each query is a pair [start, end], which means decrementing all elements from index start to end in nums.
+	•	To represent this using diff:
+	•	Increment diff[start] by 1 to indicate the beginning of a decrement operation.
+	•	Decrement diff[end + 1] by 1 to indicate the end of a decrement operation.
+	•	This approach efficiently accumulates operations in diff without updating nums directly for each query.
+	3.	Check if We Can Make All Elements Zero:
+	•	We maintain a running sum ops to accumulate the effects of all decrement operations using diff.
+	•	For each element in nums, we add diff[i] to ops to get the total operations that can be applied up to index i.
+	•	If at any point ops (the number of operations we have so far) is less than nums[i], we cannot decrement nums[i] to zero, and we return False.
+	•	If all elements can be decremented to zero, we return True.</t>
+  </si>
+  <si>
+    <t>Time: O(N+Q)
+Space: O(N)</t>
+  </si>
+  <si>
+    <t>Zero Array Transformation I</t>
+  </si>
+  <si>
+    <t>Q2(11/17/2024)</t>
+  </si>
+  <si>
+    <t>Q3(11/17/2024)</t>
+  </si>
+  <si>
+    <t>Zero Array Transformation II</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def minZeroArray(self, nums: List[int], queries: List[List[int]]) -&gt; int:
+        def works(k):
+            diff = [0] * (len(nums) + 1)
+            for l, r, v in (queries[:k]):
+                diff[l] += v
+                diff[r+1] -= v
+            for i in range(1, len(diff)):
+                diff[i] += diff[i-1]
+            for i in range(len(nums)):
+                if diff[i] &lt; nums[i]:
+                    return False
+            return True
+        ans = len(queries)+1
+        L = 0
+        R = len(queries)+1
+        while L &lt; R:
+            M = (L+R)//2
+            if works(M):
+                # can reduce K
+                R = M
+                ans = min(ans, M)
+            else:
+                L = M+1
+        if ans == len(queries)+1:
+            return -1
+        return ans</t>
+  </si>
+  <si>
+    <t>1.	Function works(k):
+	•	This function checks if the first k queries can make all elements of nums zero or less.
+	•	It uses a difference array technique to apply increment operations efficiently:
+	•	diff is an auxiliary array used to keep track of how many times each element of nums should be incremented.
+	•	For each query (l, r, v) up to the k-th query:
+	•	diff[l] += v: Start incrementing from index l.
+	•	diff[r + 1] -= v: Stop incrementing after index r.
+	•	A prefix sum on diff is calculated to get the final increments for each index in nums.
+	•	The loop then checks if all elements in nums can be made zero or less using these increments:
+	•	If any element in nums is still greater than the corresponding value in diff, works(k) returns False.
+	•	Otherwise, it returns True.
+	2.	Binary Search Logic:
+	•	The goal is to find the minimum number of queries k that can make all elements of nums zero or less.
+	•	Binary Search:
+	•	L is initialized to 0, and R to len(queries) + 1 to search for the minimum valid k.
+	•	M = (L + R) // 2 is the midpoint used to test the number of queries.
+	•	If works(M) returns True, it means M queries are sufficient, and we try to reduce k by setting R = M and updating ans.
+	•	If works(M) returns False, it means M queries are not enough, and we increase k by setting L = M + 1.
+	•	If ans remains equal to len(queries) + 1, it means it was impossible to make all elements zero, so the function returns -1.
+	•	Otherwise, it returns ans, the minimum number of queries required.</t>
+  </si>
+  <si>
+    <t>Time: O(N+M * log(M))
+Space: O(N)</t>
   </si>
 </sst>
 </file>
@@ -7836,8 +7952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+    <sheetView tabSelected="1" topLeftCell="A237" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F237" sqref="F237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.6640625" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -24763,13 +24879,25 @@
       <c r="BP235" s="8"/>
       <c r="BQ235" s="8"/>
     </row>
-    <row r="236" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A236" s="8"/>
-      <c r="B236" s="8"/>
-      <c r="C236" s="8"/>
-      <c r="D236" s="8"/>
-      <c r="E236" s="8"/>
-      <c r="F236" s="8"/>
+    <row r="236" spans="1:69" ht="395" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>871</v>
+      </c>
       <c r="G236" s="8"/>
       <c r="H236" s="8"/>
       <c r="I236" s="8"/>
@@ -24834,13 +24962,25 @@
       <c r="BP236" s="8"/>
       <c r="BQ236" s="8"/>
     </row>
-    <row r="237" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A237" s="8"/>
-      <c r="B237" s="8"/>
-      <c r="C237" s="8"/>
-      <c r="D237" s="8"/>
-      <c r="E237" s="8"/>
-      <c r="F237" s="8"/>
+    <row r="237" spans="1:69" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>878</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>879</v>
+      </c>
       <c r="G237" s="8"/>
       <c r="H237" s="8"/>
       <c r="I237" s="8"/>

</xml_diff>